<commit_message>
Add index with filtered codes
</commit_message>
<xml_diff>
--- a/data/icd9.xlsx
+++ b/data/icd9.xlsx
@@ -459,8 +459,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -480,7 +482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -488,6 +490,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -495,6 +498,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -827,7 +831,7 @@
   <dimension ref="A1:F64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>